<commit_message>
Update and simplify example files
Also fixes a typo in the template.
</commit_message>
<xml_diff>
--- a/src/voc4cat/blank_043.xlsx
+++ b/src/voc4cat/blank_043.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dlinke\MyProg_local\gh-nfdi4cat\voc4cat-tool\src\voc4cat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A4E311F-0E89-4D32-9401-02D9BB6D8E63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{394D52E2-E415-4DB8-A846-0732F18FA77D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="652" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="652" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" r:id="rId1"/>
@@ -177,9 +177,6 @@
     <t>Namespace</t>
   </si>
   <si>
-    <t>Required: URI or CURI</t>
-  </si>
-  <si>
     <t>Collection IRI</t>
   </si>
   <si>
@@ -244,9 +241,6 @@
   </si>
   <si>
     <t>Date of creation</t>
-  </si>
-  <si>
-    <t>IRI or CURI for this vocabulary</t>
   </si>
   <si>
     <t>Title of the vocabulary</t>
@@ -1474,6 +1468,12 @@
   </si>
   <si>
     <t>https://github.com/nfdi4cat/???/issues</t>
+  </si>
+  <si>
+    <t>IRI or CURIE for this vocabulary</t>
+  </si>
+  <si>
+    <t>Required: URI or CURIE</t>
   </si>
 </sst>
 </file>
@@ -2312,7 +2312,7 @@
   </sheetPr>
   <dimension ref="A11:L31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B14" sqref="B14:J18"/>
     </sheetView>
   </sheetViews>
@@ -2331,7 +2331,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="3"/>
       <c r="I11" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J11" s="7" t="s">
         <v>0</v>
@@ -2340,15 +2340,15 @@
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H12" s="24"/>
       <c r="I12" s="25" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="J12" s="26" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B14" s="27" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C14" s="27"/>
       <c r="D14" s="27"/>
@@ -2409,31 +2409,31 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D22" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D23" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D24" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -2441,29 +2441,29 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D26" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D27" s="8"/>
       <c r="E27" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D31" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -2490,8 +2490,8 @@
   </sheetPr>
   <dimension ref="A1:J1170"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView showGridLines="0" topLeftCell="A98" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B131" sqref="B131:J141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2499,12 +2499,12 @@
     <row r="1" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11"/>
       <c r="B1" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="27" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C2" s="27"/>
       <c r="D2" s="27"/>
@@ -2572,7 +2572,7 @@
     </row>
     <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B8" s="20" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -2585,10 +2585,10 @@
     <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B9" s="20"/>
       <c r="C9" s="21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F9" s="10"/>
       <c r="G9" s="5"/>
@@ -2598,10 +2598,10 @@
     </row>
     <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="C10" s="21" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F10" s="10"/>
       <c r="G10" s="5"/>
@@ -2622,7 +2622,7 @@
     </row>
     <row r="12" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B12" s="27" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C12" s="27"/>
       <c r="D12" s="27"/>
@@ -2997,7 +2997,7 @@
     </row>
     <row r="46" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B46" s="27" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C46" s="27"/>
       <c r="D46" s="27"/>
@@ -3451,7 +3451,7 @@
     <row r="87" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
     <row r="88" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B88" s="27" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C88" s="27"/>
       <c r="D88" s="27"/>
@@ -3751,7 +3751,7 @@
     <row r="115" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
     <row r="116" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B116" s="27" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C116" s="27"/>
       <c r="D116" s="27"/>
@@ -3908,7 +3908,7 @@
     <row r="130" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
     <row r="131" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B131" s="27" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C131" s="27"/>
       <c r="D131" s="27"/>
@@ -4032,7 +4032,7 @@
     <row r="142" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
     <row r="143" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B143" s="28" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C143" s="28"/>
       <c r="D143" s="28"/>
@@ -4089,18 +4089,18 @@
     </row>
     <row r="148" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="D148" s="21" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E148" s="10" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="149" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="D149" s="21" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E149" s="10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="150" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
@@ -5182,8 +5182,8 @@
   </sheetPr>
   <dimension ref="A1:D994"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5191,12 +5191,12 @@
     <col min="1" max="1" width="18.42578125" customWidth="1"/>
     <col min="2" max="2" width="64.140625" customWidth="1"/>
     <col min="3" max="3" width="49" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
@@ -5205,10 +5205,10 @@
       </c>
       <c r="B2" s="17"/>
       <c r="C2" s="13" t="s">
-        <v>51</v>
+        <v>84</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>28</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="39" customHeight="1" x14ac:dyDescent="0.25">
@@ -5217,7 +5217,7 @@
       </c>
       <c r="B3" s="22"/>
       <c r="C3" s="13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>3</v>
@@ -5229,7 +5229,7 @@
       </c>
       <c r="B4" s="17"/>
       <c r="C4" s="13" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>3</v>
@@ -5241,10 +5241,10 @@
       </c>
       <c r="B5" s="16"/>
       <c r="C5" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5253,10 +5253,10 @@
       </c>
       <c r="B6" s="16"/>
       <c r="C6" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5265,10 +5265,10 @@
       </c>
       <c r="B7" s="17"/>
       <c r="C7" s="13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5277,10 +5277,10 @@
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
@@ -5289,7 +5289,7 @@
       </c>
       <c r="B9" s="19"/>
       <c r="C9" s="13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>10</v>
@@ -6345,7 +6345,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -6356,19 +6356,19 @@
         <v>19</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>20</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>11</v>
@@ -6604,7 +6604,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.25">
@@ -6612,19 +6612,19 @@
         <v>18</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.25">
@@ -7149,7 +7149,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>24</v>
@@ -7158,7 +7158,7 @@
         <v>25</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
Update xlsx-templates & examples
</commit_message>
<xml_diff>
--- a/src/voc4cat/blank_043.xlsx
+++ b/src/voc4cat/blank_043.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dlinke\MyProg_local\gh-nfdi4cat\voc4cat-tool\src\voc4cat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{394D52E2-E415-4DB8-A846-0732F18FA77D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53875CC4-7B06-47A3-BFF3-BE38EA413C3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="652" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="652" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" r:id="rId1"/>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="87">
   <si>
     <t>0.4.3</t>
   </si>
@@ -111,9 +111,6 @@
     <t>Created Date*</t>
   </si>
   <si>
-    <t>Modified Date*</t>
-  </si>
-  <si>
     <t>Creator*</t>
   </si>
   <si>
@@ -138,9 +135,6 @@
     <t>Vocabulary Content Manager</t>
   </si>
   <si>
-    <t>Optional</t>
-  </si>
-  <si>
     <t>Catalogue PID</t>
   </si>
   <si>
@@ -207,9 +201,6 @@
     <t>examples of filled-out templates</t>
   </si>
   <si>
-    <t>https://surroundaustralia.github.io/vocpub-profile/specification.html</t>
-  </si>
-  <si>
     <t>SKOS RDF data produced or consumed by with voc4cat are validated against the VocPub profile using SHACL.</t>
   </si>
   <si>
@@ -237,9 +228,6 @@
     <t>Required: Date</t>
   </si>
   <si>
-    <t>Date of last modification</t>
-  </si>
-  <si>
     <t>Date of creation</t>
   </si>
   <si>
@@ -283,6 +271,9 @@
   </si>
   <si>
     <t>template-related</t>
+  </si>
+  <si>
+    <t>https://github.com/nfdi4cat/voc4cat/issues</t>
   </si>
   <si>
     <t>https://github.com/nfdi4cat/voc4cat-template/issues</t>
@@ -338,9 +329,6 @@
     <t>If you need help, feel free to create issues on github for your questions.</t>
   </si>
   <si>
-    <t>Version specifier for the vocabulary</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -535,12 +523,34 @@
       <rPr>
         <b/>
         <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Collections (optional)</t>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Finally...</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+After completing this sheet, you can process it locally with the voc4cat command line tool. To get more information about how to install and use it, visit https://github.com/nfdi4cat/voc4cat-tool/. Alteratively you may want to submit the xlsx file as a pull request to a voc4cat-enabled repository such as</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Prefix Sheet</t>
     </r>
     <r>
       <rPr>
@@ -563,508 +573,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">Collections are an easy way to group together concepts for various purposes.
-If rows are added to the sheet, all cells must be filled out.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Preferred Label</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = A simple one-line title for the Collection.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Definition</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = The defining description of this Collection that may be longer and include line-breaks.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>M</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ember IRIs</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = A comma-separated list of the Concept IRIS of all Concepts belonging to this collection.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Provenance</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = A note on the source of this Collection</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Finally...</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-After completing this sheet, you can process it locally with the voc4cat command line tool. To get more information about how to install and use it, visit https://github.com/nfdi4cat/voc4cat-tool/. Alteratively you may want to submit the xlsx file as a pull request to a voc4cat-enabled repository such as</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Concept Scheme (mandatory)</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">The Concept Scheme sheet collects the top level information about the vocabulary.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Vocabulary IRI* </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">= The IRI tat refers to this specific vocabulary. It must be a valid URI. For testing you can first use a fake value, as long as it's a valid URI, and replae it later (e.g. http://example.com/def/v1 ). 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Note: An IRI (International Resource Identifier) is like a URI (Uniform Reference Identifier) but with more permissible characters. Note: Instead of a full IRI you can use a CURIE (compact URI) defined with the prefix sheet, e.g. ex:v1 where "ex" stands for the namespace "http://example.com/def/". See below for more on te Prefix Sheet.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Title*</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> =  A short one line title for the vocabulary.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Description*</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = A general description for the vocabulary and its scope. This can be as long as needed and may contain all possible characters and line breaks.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Created Date*</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = The vocabulary's creation date.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Modified Date</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = The vocabulary's latest modification date.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Note: Dates in these cells must be recognized as date by Excel but may be in localized format.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Creator*</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = The ID of an organisation e.g. "GA". 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Publisher*</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = The ID of an organisation e.g. "CGI".
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Note: Either the abbreviation for an organisation or its full name can be given. The organisation is validated against a predefined list of organisations. If you miss an organisation, create an issue at https://github.com/nfdi4cat/vocexcel/issues and ask for addition.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Version</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = A version specifier for this vocabulary, e.g. v2022-02-22 (it is suggested to use calendar-based vesioning)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Provenance*</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = A note on the source of this vocabulary.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Custodian</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = The person managing this vocabulary's content, e.g. "Sofia Garcia (orcid:0000-0001-2345-6789)"
-</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Catalogue PID</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = A catalogue PID or DOI, e.g. eCat ID, if the vocab has one.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Prefix Sheet</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>This sheet is for defining a mapping between short pefixes and namespaces which are the basis for using "compact URI" also called "CURIE". For more on compact URIs, see https://www.w3.org/TR/2010/NOTE-curie-20101216/
 Example</t>
     </r>
@@ -1134,6 +642,15 @@
   </si>
   <si>
     <t>revision</t>
+  </si>
+  <si>
+    <t>Concepts*</t>
+  </si>
+  <si>
+    <t>IRI or CURIE for this vocabulary</t>
+  </si>
+  <si>
+    <t>Required: URI or CURIE</t>
   </si>
   <si>
     <r>
@@ -1427,7 +944,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> = A note on the source of this Concept
+      <t xml:space="preserve"> = A note on the source of this Concept; see above for what is expected in provenance fields.
 </t>
     </r>
     <r>
@@ -1461,19 +978,527 @@
     </r>
   </si>
   <si>
-    <t>Concepts*</t>
-  </si>
-  <si>
-    <t>2023-06a</t>
-  </si>
-  <si>
-    <t>https://github.com/nfdi4cat/???/issues</t>
-  </si>
-  <si>
-    <t>IRI or CURIE for this vocabulary</t>
-  </si>
-  <si>
-    <t>Required: URI or CURIE</t>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Collections (optional)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Collections are an easy way to group together concepts for various purposes.
+If rows are added to the sheet, all cells must be filled out.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Preferred Label</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = A simple one-line title for the Collection.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Definition</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = The defining description of this Collection that may be longer and include line-breaks.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>M</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ember IRIs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = A comma-separated list of the Concept IRIS of all Concepts belonging to this collection.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Provenance</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = A note on the source of this Collection; see above for what is expected in provenance fields.</t>
+    </r>
+  </si>
+  <si>
+    <t>2023-08b</t>
+  </si>
+  <si>
+    <t>https://w3id.org/profile/vocpub</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Concept Scheme (mandatory)</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">The Concept Scheme sheet collects the top level information about the vocabulary.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Vocabulary IRI* </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">= The IRI tat refers to this specific vocabulary. It must be a valid URI. For testing you can first use a fake value, as long as it's a valid URI, and replae it later (e.g. http://example.com/def/v1 ). 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Note: An IRI (International Resource Identifier) is like a URI (Uniform Reference Identifier) but with more permissible characters. Note: Instead of a full IRI you can use a CURIE (compact URI) defined with the prefix sheet, e.g. ex:v1 where "ex" stands for the namespace "http://example.com/def/". See below for more on te Prefix Sheet.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Title*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> =  A short one line title for the vocabulary.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Description*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = A general description for the vocabulary and its scope. This can be as long as needed and may contain all possible characters and line breaks.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Created Date*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = The vocabulary's creation date.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Modified Date</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = The vocabulary's latest modification date (optional).
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Note: Dates in these cells must be recognized as date by Excel but may be in localized format.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Creator*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = A ROR ID, an ORCID or a predefined short-ID-string for an organisation, e.g. "NFDI4Cat". 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Publisher*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = A ROR ID or a predefined short-ID-string for an organisation, e.g. "NFDI4Cat". 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Note: Either the abbreviation for an organisation or its URI can be given. The organisation abbreviation is validated against a predefined list of organisations. If you miss an organisation, create an issue at https://github.com/nfdi4cat/vocexcel/issues and ask for addition (or just use a ROR ID!).</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Version</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = A version specifier for this vocabulary, e.g. v2022-02-22 (it is suggested to use calendar-based vesioning).
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Note: Versions strings should start with "v" to prevent Excel from interpreting it as number of date.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Provenance*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = A note on the source of this vocabulary. This should be an identifier for the person and a provenance note. As identifier, an ORCID ID (with or without https://orcid.org/ part) or a github name should be used. Multiple entries must be seperated with a comma. For provenance fields there is no strict validation in place because handling of provenance is still in discussion, see https://github.com/nfdi4cat/voc4cat-tool/issues/122
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Custodian</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = The person managing this vocabulary's content, e.g. "Sofia Garcia (orcid:0000-0001-2345-6789)"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Catalogue PID</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = A catalogue PID or DOI, e.g. eCat ID, if the vocab has one.</t>
+    </r>
+  </si>
+  <si>
+    <t>Optional: Date</t>
+  </si>
+  <si>
+    <t>Version specifier for the vocabulary (or empty cell)</t>
+  </si>
+  <si>
+    <t>Date of last modification (or empty cell)</t>
+  </si>
+  <si>
+    <t>Modified Date</t>
+  </si>
+  <si>
+    <t>Optional: URI or Text</t>
   </si>
 </sst>
 </file>
@@ -1952,6 +1977,63 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Grafik 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+            <a:ext uri="{C183D7F6-B498-43B3-948B-1728B52AA6E4}">
+              <adec:decorative xmlns:adec="http://schemas.microsoft.com/office/drawing/2017/decorative" val="1"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect t="32488" b="34619"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1095375" y="304800"/>
+          <a:ext cx="4514850" cy="1543050"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8DAB75F9-D01E-4902-B5DF-39342F86B90D}" name="concepts" displayName="concepts" ref="A2:I20" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
   <autoFilter ref="A2:I20" xr:uid="{8DAB75F9-D01E-4902-B5DF-39342F86B90D}"/>
@@ -2000,8 +2082,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{0A8562A3-BEFF-43D4-B887-56FC0330A95A}" name="prefixes" displayName="prefixes" ref="A1:B20" totalsRowShown="0" headerRowDxfId="6">
-  <autoFilter ref="A1:B20" xr:uid="{0A8562A3-BEFF-43D4-B887-56FC0330A95A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{0A8562A3-BEFF-43D4-B887-56FC0330A95A}" name="prefixes" displayName="prefixes" ref="A1:B19" totalsRowShown="0" headerRowDxfId="6">
+  <autoFilter ref="A1:B19" xr:uid="{0A8562A3-BEFF-43D4-B887-56FC0330A95A}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{A30D4DF8-3B4A-4F43-9882-EDFDD8090F9E}" name="Prefix"/>
     <tableColumn id="2" xr3:uid="{6285A3D9-0152-4BE7-AC6A-AF758EEFAF51}" name="Namespace"/>
@@ -2312,8 +2394,8 @@
   </sheetPr>
   <dimension ref="A11:L31"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14:J18"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2331,7 +2413,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="3"/>
       <c r="I11" s="6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="J11" s="7" t="s">
         <v>0</v>
@@ -2340,15 +2422,15 @@
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H12" s="24"/>
       <c r="I12" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="J12" s="26" t="s">
         <v>79</v>
-      </c>
-      <c r="J12" s="26" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B14" s="27" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C14" s="27"/>
       <c r="D14" s="27"/>
@@ -2409,31 +2491,31 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D22" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D23" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D24" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -2441,29 +2523,29 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D26" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D27" s="8"/>
       <c r="E27" s="10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D31" s="8" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>38</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -2480,6 +2562,7 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
+  <drawing r:id="rId8"/>
 </worksheet>
 </file>
 
@@ -2488,10 +2571,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J1170"/>
+  <dimension ref="A1:J1172"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A98" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B131" sqref="B131:J141"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48:J88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2499,12 +2582,12 @@
     <row r="1" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11"/>
       <c r="B1" s="11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="27" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C2" s="27"/>
       <c r="D2" s="27"/>
@@ -2572,7 +2655,7 @@
     </row>
     <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B8" s="20" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -2585,10 +2668,10 @@
     <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B9" s="20"/>
       <c r="C9" s="21" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="F9" s="10"/>
       <c r="G9" s="5"/>
@@ -2598,10 +2681,10 @@
     </row>
     <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="C10" s="21" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F10" s="10"/>
       <c r="G10" s="5"/>
@@ -2622,7 +2705,7 @@
     </row>
     <row r="12" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B12" s="27" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C12" s="27"/>
       <c r="D12" s="27"/>
@@ -2986,19 +3069,18 @@
       <c r="J44" s="27"/>
     </row>
     <row r="45" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="C45" s="5"/>
-      <c r="D45" s="5"/>
-      <c r="E45" s="5"/>
-      <c r="F45" s="5"/>
-      <c r="G45" s="5"/>
-      <c r="H45" s="5"/>
-      <c r="I45" s="5"/>
-      <c r="J45" s="5"/>
+      <c r="B45" s="27"/>
+      <c r="C45" s="27"/>
+      <c r="D45" s="27"/>
+      <c r="E45" s="27"/>
+      <c r="F45" s="27"/>
+      <c r="G45" s="27"/>
+      <c r="H45" s="27"/>
+      <c r="I45" s="27"/>
+      <c r="J45" s="27"/>
     </row>
     <row r="46" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B46" s="27" t="s">
-        <v>80</v>
-      </c>
+      <c r="B46" s="27"/>
       <c r="C46" s="27"/>
       <c r="D46" s="27"/>
       <c r="E46" s="27"/>
@@ -3009,18 +3091,19 @@
       <c r="J46" s="27"/>
     </row>
     <row r="47" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B47" s="27"/>
-      <c r="C47" s="27"/>
-      <c r="D47" s="27"/>
-      <c r="E47" s="27"/>
-      <c r="F47" s="27"/>
-      <c r="G47" s="27"/>
-      <c r="H47" s="27"/>
-      <c r="I47" s="27"/>
-      <c r="J47" s="27"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="5"/>
+      <c r="F47" s="5"/>
+      <c r="G47" s="5"/>
+      <c r="H47" s="5"/>
+      <c r="I47" s="5"/>
+      <c r="J47" s="5"/>
     </row>
     <row r="48" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B48" s="27"/>
+      <c r="B48" s="27" t="s">
+        <v>77</v>
+      </c>
       <c r="C48" s="27"/>
       <c r="D48" s="27"/>
       <c r="E48" s="27"/>
@@ -3448,11 +3531,19 @@
       <c r="I86" s="27"/>
       <c r="J86" s="27"/>
     </row>
-    <row r="87" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="87" spans="2:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="B87" s="27"/>
+      <c r="C87" s="27"/>
+      <c r="D87" s="27"/>
+      <c r="E87" s="27"/>
+      <c r="F87" s="27"/>
+      <c r="G87" s="27"/>
+      <c r="H87" s="27"/>
+      <c r="I87" s="27"/>
+      <c r="J87" s="27"/>
+    </row>
     <row r="88" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B88" s="27" t="s">
-        <v>74</v>
-      </c>
+      <c r="B88" s="27"/>
       <c r="C88" s="27"/>
       <c r="D88" s="27"/>
       <c r="E88" s="27"/>
@@ -3462,19 +3553,11 @@
       <c r="I88" s="27"/>
       <c r="J88" s="27"/>
     </row>
-    <row r="89" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B89" s="27"/>
-      <c r="C89" s="27"/>
-      <c r="D89" s="27"/>
-      <c r="E89" s="27"/>
-      <c r="F89" s="27"/>
-      <c r="G89" s="27"/>
-      <c r="H89" s="27"/>
-      <c r="I89" s="27"/>
-      <c r="J89" s="27"/>
-    </row>
+    <row r="89" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
     <row r="90" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B90" s="27"/>
+      <c r="B90" s="27" t="s">
+        <v>70</v>
+      </c>
       <c r="C90" s="27"/>
       <c r="D90" s="27"/>
       <c r="E90" s="27"/>
@@ -3748,11 +3831,19 @@
       <c r="I114" s="27"/>
       <c r="J114" s="27"/>
     </row>
-    <row r="115" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="115" spans="2:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="B115" s="27"/>
+      <c r="C115" s="27"/>
+      <c r="D115" s="27"/>
+      <c r="E115" s="27"/>
+      <c r="F115" s="27"/>
+      <c r="G115" s="27"/>
+      <c r="H115" s="27"/>
+      <c r="I115" s="27"/>
+      <c r="J115" s="27"/>
+    </row>
     <row r="116" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B116" s="27" t="s">
-        <v>75</v>
-      </c>
+      <c r="B116" s="27"/>
       <c r="C116" s="27"/>
       <c r="D116" s="27"/>
       <c r="E116" s="27"/>
@@ -3762,19 +3853,11 @@
       <c r="I116" s="27"/>
       <c r="J116" s="27"/>
     </row>
-    <row r="117" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B117" s="27"/>
-      <c r="C117" s="27"/>
-      <c r="D117" s="27"/>
-      <c r="E117" s="27"/>
-      <c r="F117" s="27"/>
-      <c r="G117" s="27"/>
-      <c r="H117" s="27"/>
-      <c r="I117" s="27"/>
-      <c r="J117" s="27"/>
-    </row>
+    <row r="117" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
     <row r="118" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B118" s="27"/>
+      <c r="B118" s="27" t="s">
+        <v>78</v>
+      </c>
       <c r="C118" s="27"/>
       <c r="D118" s="27"/>
       <c r="E118" s="27"/>
@@ -3905,11 +3988,19 @@
       <c r="I129" s="27"/>
       <c r="J129" s="27"/>
     </row>
-    <row r="130" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="130" spans="2:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="B130" s="27"/>
+      <c r="C130" s="27"/>
+      <c r="D130" s="27"/>
+      <c r="E130" s="27"/>
+      <c r="F130" s="27"/>
+      <c r="G130" s="27"/>
+      <c r="H130" s="27"/>
+      <c r="I130" s="27"/>
+      <c r="J130" s="27"/>
+    </row>
     <row r="131" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B131" s="27" t="s">
-        <v>78</v>
-      </c>
+      <c r="B131" s="27"/>
       <c r="C131" s="27"/>
       <c r="D131" s="27"/>
       <c r="E131" s="27"/>
@@ -3919,19 +4010,11 @@
       <c r="I131" s="27"/>
       <c r="J131" s="27"/>
     </row>
-    <row r="132" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B132" s="27"/>
-      <c r="C132" s="27"/>
-      <c r="D132" s="27"/>
-      <c r="E132" s="27"/>
-      <c r="F132" s="27"/>
-      <c r="G132" s="27"/>
-      <c r="H132" s="27"/>
-      <c r="I132" s="27"/>
-      <c r="J132" s="27"/>
-    </row>
+    <row r="132" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
     <row r="133" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B133" s="27"/>
+      <c r="B133" s="27" t="s">
+        <v>72</v>
+      </c>
       <c r="C133" s="27"/>
       <c r="D133" s="27"/>
       <c r="E133" s="27"/>
@@ -4029,33 +4112,33 @@
       <c r="I141" s="27"/>
       <c r="J141" s="27"/>
     </row>
-    <row r="142" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="142" spans="2:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="B142" s="27"/>
+      <c r="C142" s="27"/>
+      <c r="D142" s="27"/>
+      <c r="E142" s="27"/>
+      <c r="F142" s="27"/>
+      <c r="G142" s="27"/>
+      <c r="H142" s="27"/>
+      <c r="I142" s="27"/>
+      <c r="J142" s="27"/>
+    </row>
     <row r="143" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B143" s="28" t="s">
-        <v>76</v>
-      </c>
-      <c r="C143" s="28"/>
-      <c r="D143" s="28"/>
-      <c r="E143" s="28"/>
-      <c r="F143" s="28"/>
-      <c r="G143" s="28"/>
-      <c r="H143" s="28"/>
-      <c r="I143" s="28"/>
-      <c r="J143" s="28"/>
-    </row>
-    <row r="144" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B144" s="28"/>
-      <c r="C144" s="28"/>
-      <c r="D144" s="28"/>
-      <c r="E144" s="28"/>
-      <c r="F144" s="28"/>
-      <c r="G144" s="28"/>
-      <c r="H144" s="28"/>
-      <c r="I144" s="28"/>
-      <c r="J144" s="28"/>
-    </row>
+      <c r="B143" s="27"/>
+      <c r="C143" s="27"/>
+      <c r="D143" s="27"/>
+      <c r="E143" s="27"/>
+      <c r="F143" s="27"/>
+      <c r="G143" s="27"/>
+      <c r="H143" s="27"/>
+      <c r="I143" s="27"/>
+      <c r="J143" s="27"/>
+    </row>
+    <row r="144" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
     <row r="145" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B145" s="28"/>
+      <c r="B145" s="28" t="s">
+        <v>71</v>
+      </c>
       <c r="C145" s="28"/>
       <c r="D145" s="28"/>
       <c r="E145" s="28"/>
@@ -4088,23 +4171,43 @@
       <c r="J147" s="28"/>
     </row>
     <row r="148" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="D148" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="E148" s="10" t="s">
-        <v>68</v>
-      </c>
+      <c r="B148" s="28"/>
+      <c r="C148" s="28"/>
+      <c r="D148" s="28"/>
+      <c r="E148" s="28"/>
+      <c r="F148" s="28"/>
+      <c r="G148" s="28"/>
+      <c r="H148" s="28"/>
+      <c r="I148" s="28"/>
+      <c r="J148" s="28"/>
     </row>
     <row r="149" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="D149" s="21" t="s">
+      <c r="B149" s="28"/>
+      <c r="C149" s="28"/>
+      <c r="D149" s="28"/>
+      <c r="E149" s="28"/>
+      <c r="F149" s="28"/>
+      <c r="G149" s="28"/>
+      <c r="H149" s="28"/>
+      <c r="I149" s="28"/>
+      <c r="J149" s="28"/>
+    </row>
+    <row r="150" spans="2:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="D150" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="E150" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="151" spans="2:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="D151" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="E151" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="E149" s="10" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="150" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="151" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
+    </row>
     <row r="152" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
     <row r="153" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
     <row r="154" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
@@ -5124,51 +5227,53 @@
     <row r="1168" ht="15" x14ac:dyDescent="0.25"/>
     <row r="1169" ht="15" x14ac:dyDescent="0.25"/>
     <row r="1170" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="1171" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="1172" ht="15" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="B131:J141"/>
-    <mergeCell ref="B143:J147"/>
+    <mergeCell ref="B133:J143"/>
+    <mergeCell ref="B145:J149"/>
     <mergeCell ref="B2:J6"/>
-    <mergeCell ref="B12:J44"/>
-    <mergeCell ref="B46:J86"/>
-    <mergeCell ref="B88:J114"/>
-    <mergeCell ref="B116:J129"/>
+    <mergeCell ref="B12:J46"/>
+    <mergeCell ref="B48:J88"/>
+    <mergeCell ref="B90:J116"/>
+    <mergeCell ref="B118:J131"/>
   </mergeCells>
-  <conditionalFormatting sqref="B2:B4 B46:B86">
+  <conditionalFormatting sqref="B2:B4 B48:B88">
     <cfRule type="containsBlanks" dxfId="5" priority="7">
       <formula>LEN(TRIM(B2))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B12:B44">
+  <conditionalFormatting sqref="B12:B46">
     <cfRule type="containsBlanks" dxfId="4" priority="6">
       <formula>LEN(TRIM(B12))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B88">
+  <conditionalFormatting sqref="B90">
     <cfRule type="containsBlanks" dxfId="3" priority="4">
-      <formula>LEN(TRIM(B88))=0</formula>
+      <formula>LEN(TRIM(B90))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B116">
+  <conditionalFormatting sqref="B118">
     <cfRule type="containsBlanks" dxfId="2" priority="3">
-      <formula>LEN(TRIM(B116))=0</formula>
+      <formula>LEN(TRIM(B118))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B131">
+  <conditionalFormatting sqref="B133">
     <cfRule type="containsBlanks" dxfId="1" priority="2">
-      <formula>LEN(TRIM(B131))=0</formula>
+      <formula>LEN(TRIM(B133))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B143:B147">
+  <conditionalFormatting sqref="B145:B149">
     <cfRule type="containsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(B143))=0</formula>
+      <formula>LEN(TRIM(B145))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="D10" r:id="rId1" xr:uid="{57547A46-992F-4B46-8DCE-6851DE974B0D}"/>
     <hyperlink ref="D9" r:id="rId2" xr:uid="{7DDFAC11-0287-4E46-9BC5-4CE195DD88F1}"/>
-    <hyperlink ref="E149" r:id="rId3" xr:uid="{A5C8A041-9B1E-4C57-A8AC-D56D5CF97571}"/>
-    <hyperlink ref="E148" r:id="rId4" xr:uid="{7FFAD8C3-AA0B-4A81-9A4D-A7DC6B7D6670}"/>
+    <hyperlink ref="E151" r:id="rId3" xr:uid="{A5C8A041-9B1E-4C57-A8AC-D56D5CF97571}"/>
+    <hyperlink ref="E150" r:id="rId4" xr:uid="{7FFAD8C3-AA0B-4A81-9A4D-A7DC6B7D6670}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
@@ -5182,8 +5287,8 @@
   </sheetPr>
   <dimension ref="A1:D994"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5191,12 +5296,12 @@
     <col min="1" max="1" width="18.42578125" customWidth="1"/>
     <col min="2" max="2" width="64.140625" customWidth="1"/>
     <col min="3" max="3" width="49" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
@@ -5205,10 +5310,10 @@
       </c>
       <c r="B2" s="17"/>
       <c r="C2" s="13" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="39" customHeight="1" x14ac:dyDescent="0.25">
@@ -5217,7 +5322,7 @@
       </c>
       <c r="B3" s="22"/>
       <c r="C3" s="13" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>3</v>
@@ -5229,7 +5334,7 @@
       </c>
       <c r="B4" s="17"/>
       <c r="C4" s="13" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>3</v>
@@ -5241,67 +5346,67 @@
       </c>
       <c r="B5" s="16"/>
       <c r="C5" s="13" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>6</v>
+        <v>85</v>
       </c>
       <c r="B6" s="16"/>
       <c r="C6" s="13" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>47</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="17"/>
       <c r="C7" s="13" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="17"/>
       <c r="C8" s="13" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="19"/>
       <c r="C9" s="13" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" s="17"/>
       <c r="C10" s="13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>3</v>
@@ -5309,26 +5414,26 @@
     </row>
     <row r="11" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11" s="17"/>
       <c r="C11" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B12" s="18"/>
       <c r="C12" s="13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>15</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.25"/>
@@ -6345,36 +6450,36 @@
   <sheetData>
     <row r="1" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -6396,8 +6501,8 @@
       <c r="E4" s="12"/>
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="23"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="12"/>
@@ -6604,27 +6709,27 @@
   <sheetData>
     <row r="1" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.25">
@@ -7144,24 +7249,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -7317,15 +7422,15 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="custom" allowBlank="1" showErrorMessage="1" errorTitle="Prefix ends with colon" error="A prefix may not end with a colon(:)!" sqref="A2:A20" xr:uid="{3E636239-7DFF-4815-80F6-149A9A69419E}">
+    <dataValidation type="custom" allowBlank="1" showErrorMessage="1" errorTitle="Prefix ends with colon" error="A prefix may not end with a colon(:)!" sqref="A2:A19" xr:uid="{3E636239-7DFF-4815-80F6-149A9A69419E}">
       <formula1>ISERROR(SEARCH(":",A2))</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Adapt help for prefix-sheet & adjust default col. widths
</commit_message>
<xml_diff>
--- a/src/voc4cat/blank_043.xlsx
+++ b/src/voc4cat/blank_043.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dlinke\MyProg_local\gh-nfdi4cat\voc4cat-tool\src\voc4cat\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\MyProg\gh-nfdi4cat\voc4cat-tool\src\voc4cat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53875CC4-7B06-47A3-BFF3-BE38EA413C3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A831E59-7952-40F5-BC3E-7B5EE32B40F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="652" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="300" yWindow="2340" windowWidth="28500" windowHeight="14700" tabRatio="652" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" r:id="rId1"/>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="88">
   <si>
     <t>0.4.3</t>
   </si>
@@ -538,106 +538,6 @@
       </rPr>
       <t xml:space="preserve">
 After completing this sheet, you can process it locally with the voc4cat command line tool. To get more information about how to install and use it, visit https://github.com/nfdi4cat/voc4cat-tool/. Alteratively you may want to submit the xlsx file as a pull request to a voc4cat-enabled repository such as</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Prefix Sheet</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>This sheet is for defining a mapping between short pefixes and namespaces which are the basis for using "compact URI" also called "CURIE". For more on compact URIs, see https://www.w3.org/TR/2010/NOTE-curie-20101216/
-Example</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: http://example.org/1, http://example.org/2, http://example.org/3</t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color rgb="FF1155CC"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Instead of manually typing out said examples, you can add in the Prefix Sheet a "ex" as Prefix, and</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> "http://example.org/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">" as the coresponding namespace. Then instead of writing the whole IRI, it is possible to write "ex:1, ex:2, ex:3".
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Note: In the Prefix Sheet the Prefix must be entered without a colon at the end. Only when the prefix is used in CURIE a colon is used to seperate the prefix from the suffix-part of the IRI.</t>
     </r>
   </si>
   <si>
@@ -1499,6 +1399,97 @@
   </si>
   <si>
     <t>Optional: URI or Text</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Prefix Sheet</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>This sheet shows the known mappings between short pefixes and namespaces which are the basis for using "compact URI" also called "CURIE". This sheet is write only; any changes will be ignored. For more on compact URIs, see https://www.w3.org/TR/2010/NOTE-curie-20101216/
+Example</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: http://example.org/1, http://example.org/2, http://example.org/3</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF1155CC"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Instead of manually typing out said examples, you can add in the Prefix Sheet a "ex" as Prefix, and</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "http://example.org/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" as the coresponding namespace. Then instead of writing the whole IRI, it is possible to write "ex:1, ex:2, ex:3".</t>
+    </r>
+  </si>
+  <si>
+    <t>voc4cat_0000194</t>
   </si>
 </sst>
 </file>
@@ -2093,9 +2084,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 – 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2133,7 +2124,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 – 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2239,7 +2230,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 – 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2381,7 +2372,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2394,7 +2385,7 @@
   </sheetPr>
   <dimension ref="A11:L31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
@@ -2422,10 +2413,10 @@
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H12" s="24"/>
       <c r="I12" s="25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J12" s="26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -2545,7 +2536,7 @@
         <v>37</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -2571,10 +2562,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J1172"/>
+  <dimension ref="A1:J1170"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48:J88"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2705,7 +2696,7 @@
     </row>
     <row r="12" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B12" s="27" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C12" s="27"/>
       <c r="D12" s="27"/>
@@ -3102,7 +3093,7 @@
     </row>
     <row r="48" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B48" s="27" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C48" s="27"/>
       <c r="D48" s="27"/>
@@ -3856,7 +3847,7 @@
     <row r="117" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
     <row r="118" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B118" s="27" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C118" s="27"/>
       <c r="D118" s="27"/>
@@ -4013,7 +4004,7 @@
     <row r="132" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
     <row r="133" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B133" s="27" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
       <c r="C133" s="27"/>
       <c r="D133" s="27"/>
@@ -4112,33 +4103,33 @@
       <c r="I141" s="27"/>
       <c r="J141" s="27"/>
     </row>
-    <row r="142" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B142" s="27"/>
-      <c r="C142" s="27"/>
-      <c r="D142" s="27"/>
-      <c r="E142" s="27"/>
-      <c r="F142" s="27"/>
-      <c r="G142" s="27"/>
-      <c r="H142" s="27"/>
-      <c r="I142" s="27"/>
-      <c r="J142" s="27"/>
-    </row>
+    <row r="142" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
     <row r="143" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B143" s="27"/>
-      <c r="C143" s="27"/>
-      <c r="D143" s="27"/>
-      <c r="E143" s="27"/>
-      <c r="F143" s="27"/>
-      <c r="G143" s="27"/>
-      <c r="H143" s="27"/>
-      <c r="I143" s="27"/>
-      <c r="J143" s="27"/>
-    </row>
-    <row r="144" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
+      <c r="B143" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="C143" s="28"/>
+      <c r="D143" s="28"/>
+      <c r="E143" s="28"/>
+      <c r="F143" s="28"/>
+      <c r="G143" s="28"/>
+      <c r="H143" s="28"/>
+      <c r="I143" s="28"/>
+      <c r="J143" s="28"/>
+    </row>
+    <row r="144" spans="2:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="B144" s="28"/>
+      <c r="C144" s="28"/>
+      <c r="D144" s="28"/>
+      <c r="E144" s="28"/>
+      <c r="F144" s="28"/>
+      <c r="G144" s="28"/>
+      <c r="H144" s="28"/>
+      <c r="I144" s="28"/>
+      <c r="J144" s="28"/>
+    </row>
     <row r="145" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B145" s="28" t="s">
-        <v>71</v>
-      </c>
+      <c r="B145" s="28"/>
       <c r="C145" s="28"/>
       <c r="D145" s="28"/>
       <c r="E145" s="28"/>
@@ -4171,43 +4162,23 @@
       <c r="J147" s="28"/>
     </row>
     <row r="148" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B148" s="28"/>
-      <c r="C148" s="28"/>
-      <c r="D148" s="28"/>
-      <c r="E148" s="28"/>
-      <c r="F148" s="28"/>
-      <c r="G148" s="28"/>
-      <c r="H148" s="28"/>
-      <c r="I148" s="28"/>
-      <c r="J148" s="28"/>
+      <c r="D148" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="E148" s="10" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="149" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B149" s="28"/>
-      <c r="C149" s="28"/>
-      <c r="D149" s="28"/>
-      <c r="E149" s="28"/>
-      <c r="F149" s="28"/>
-      <c r="G149" s="28"/>
-      <c r="H149" s="28"/>
-      <c r="I149" s="28"/>
-      <c r="J149" s="28"/>
-    </row>
-    <row r="150" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="D150" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="E150" s="10" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="151" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="D151" s="21" t="s">
+      <c r="D149" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="E151" s="10" t="s">
+      <c r="E149" s="10" t="s">
         <v>66</v>
       </c>
     </row>
+    <row r="150" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="151" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
     <row r="152" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
     <row r="153" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
     <row r="154" spans="2:10" ht="15" x14ac:dyDescent="0.25"/>
@@ -5227,12 +5198,10 @@
     <row r="1168" ht="15" x14ac:dyDescent="0.25"/>
     <row r="1169" ht="15" x14ac:dyDescent="0.25"/>
     <row r="1170" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="1171" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="1172" ht="15" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="B133:J143"/>
-    <mergeCell ref="B145:J149"/>
+    <mergeCell ref="B133:J141"/>
+    <mergeCell ref="B143:J147"/>
     <mergeCell ref="B2:J6"/>
     <mergeCell ref="B12:J46"/>
     <mergeCell ref="B48:J88"/>
@@ -5264,16 +5233,16 @@
       <formula>LEN(TRIM(B133))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B145:B149">
+  <conditionalFormatting sqref="B143:B147">
     <cfRule type="containsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(B145))=0</formula>
+      <formula>LEN(TRIM(B143))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="D10" r:id="rId1" xr:uid="{57547A46-992F-4B46-8DCE-6851DE974B0D}"/>
     <hyperlink ref="D9" r:id="rId2" xr:uid="{7DDFAC11-0287-4E46-9BC5-4CE195DD88F1}"/>
-    <hyperlink ref="E151" r:id="rId3" xr:uid="{A5C8A041-9B1E-4C57-A8AC-D56D5CF97571}"/>
-    <hyperlink ref="E150" r:id="rId4" xr:uid="{7FFAD8C3-AA0B-4A81-9A4D-A7DC6B7D6670}"/>
+    <hyperlink ref="E149" r:id="rId3" xr:uid="{A5C8A041-9B1E-4C57-A8AC-D56D5CF97571}"/>
+    <hyperlink ref="E148" r:id="rId4" xr:uid="{7FFAD8C3-AA0B-4A81-9A4D-A7DC6B7D6670}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
@@ -5287,14 +5256,14 @@
   </sheetPr>
   <dimension ref="A1:D994"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.42578125" customWidth="1"/>
-    <col min="2" max="2" width="64.140625" customWidth="1"/>
+    <col min="2" max="2" width="80.7109375" customWidth="1"/>
     <col min="3" max="3" width="49" customWidth="1"/>
     <col min="4" max="4" width="21.28515625" bestFit="1" customWidth="1"/>
   </cols>
@@ -5310,10 +5279,10 @@
       </c>
       <c r="B2" s="17"/>
       <c r="C2" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="D2" s="14" t="s">
         <v>75</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="39" customHeight="1" x14ac:dyDescent="0.25">
@@ -5354,14 +5323,14 @@
     </row>
     <row r="6" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B6" s="16"/>
       <c r="C6" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5394,13 +5363,13 @@
       </c>
       <c r="B9" s="19"/>
       <c r="C9" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>10</v>
       </c>
@@ -5433,7 +5402,7 @@
         <v>15</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.25"/>
@@ -6432,28 +6401,28 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.85546875" customWidth="1"/>
     <col min="2" max="2" width="36.85546875" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
     <col min="4" max="4" width="50.140625" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
     <col min="6" max="6" width="30" customWidth="1"/>
-    <col min="7" max="7" width="27" customWidth="1"/>
+    <col min="7" max="7" width="40.85546875" customWidth="1"/>
     <col min="8" max="8" width="23.5703125" customWidth="1"/>
     <col min="9" max="9" width="26.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
@@ -6483,7 +6452,9 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="12"/>
+      <c r="A3" s="12" t="s">
+        <v>87</v>
+      </c>
       <c r="B3" s="9"/>
       <c r="C3" s="12"/>
       <c r="D3" s="9"/>
@@ -6697,14 +6668,11 @@
   </sheetPr>
   <dimension ref="A1:F485"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.7109375" customWidth="1"/>
-    <col min="2" max="6" width="25.140625" customWidth="1"/>
+    <col min="1" max="6" width="40.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -7235,15 +7203,15 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="1" max="1" width="45.7109375" customWidth="1"/>
     <col min="2" max="2" width="16.85546875" customWidth="1"/>
     <col min="3" max="3" width="40.42578125" customWidth="1"/>
-    <col min="4" max="4" width="45.42578125" customWidth="1"/>
+    <col min="4" max="4" width="45.7109375" customWidth="1"/>
     <col min="5" max="5" width="26.28515625" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Remove test-entry in blank_043.xlsx
</commit_message>
<xml_diff>
--- a/src/voc4cat/blank_043.xlsx
+++ b/src/voc4cat/blank_043.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\MyProg\gh-nfdi4cat\voc4cat-tool\src\voc4cat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A831E59-7952-40F5-BC3E-7B5EE32B40F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC0AE8B4-FBD4-45A7-912B-47EE44ADA4CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="2340" windowWidth="28500" windowHeight="14700" tabRatio="652" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="300" yWindow="2340" windowWidth="28500" windowHeight="14700" tabRatio="652" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" r:id="rId1"/>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="87">
   <si>
     <t>0.4.3</t>
   </si>
@@ -1487,9 +1487,6 @@
       </rPr>
       <t>" as the coresponding namespace. Then instead of writing the whole IRI, it is possible to write "ex:1, ex:2, ex:3".</t>
     </r>
-  </si>
-  <si>
-    <t>voc4cat_0000194</t>
   </si>
 </sst>
 </file>
@@ -5256,7 +5253,7 @@
   </sheetPr>
   <dimension ref="A1:D994"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -6400,8 +6397,8 @@
   </sheetPr>
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6452,9 +6449,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
-        <v>87</v>
-      </c>
+      <c r="A3" s="12"/>
       <c r="B3" s="9"/>
       <c r="C3" s="12"/>
       <c r="D3" s="9"/>

</xml_diff>